<commit_message>
gradient descent with momentum (incl. bias issue resolved)
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17352" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
   <si>
     <t>#Iterations</t>
   </si>
@@ -276,6 +276,46 @@
       </rPr>
       <t>(1-tanh^2)</t>
     </r>
+  </si>
+  <si>
+    <t>2018.04.30</t>
+  </si>
+  <si>
+    <t>relu slightly better than tanh</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tanh*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,softmax</t>
+    </r>
+  </si>
+  <si>
+    <t>xavier did not help much, but maybe because alpha too high?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>MINIBATCHES implemented (up to here: trained on 1K data set, costs jumped between ,75 and 1,00 in last iterations</t>
   </si>
 </sst>
 </file>
@@ -649,11 +689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +707,7 @@
     <col min="8" max="8" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1290,6 +1330,143 @@
       </c>
       <c r="L18" s="8"/>
     </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>2.6</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.75608305224674899</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="8">
+        <v>2</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>2.9</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.69801583265231404</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="8">
+        <v>2</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>2.5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.85885793959385504</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="8">
+        <v>2</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>3.1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.83597837807029796</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G22" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="8">
+        <v>2</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
comaring 2 optimization techniques: 1.Gradient descent 2.Gradient descent with momentum
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t>#Iterations</t>
   </si>
@@ -316,6 +316,57 @@
   </si>
   <si>
     <t>MINIBATCHES implemented (up to here: trained on 1K data set, costs jumped between ,75 and 1,00 in last iterations</t>
+  </si>
+  <si>
+    <t>2018.05.03</t>
+  </si>
+  <si>
+    <t>Seems to optimize faster in initial 200 iterations, but later converge to similar cost</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opt technique: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gradient descent</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opt technique: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gradient descent with momentum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, beta=0,9; cost 2,2% lower; accuracy 1,6% higher after 500 iterations;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -689,11 +740,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,6 +1518,81 @@
         <v>46</v>
       </c>
     </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24">
+        <v>2.9</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1.2441706890650399</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="F24">
+        <v>500</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="8">
+        <v>2</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25">
+        <v>2.9</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1.21710047073349</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="F25">
+        <v>500</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L26" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>